<commit_message>
system tests approved by tl :)
</commit_message>
<xml_diff>
--- a/SimpCity US14 Test Document (3 Pass 0 Fail).xlsx
+++ b/SimpCity US14 Test Document (3 Pass 0 Fail).xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Tesr Documents\Sprint 4 V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D34A003-3B93-4D6E-B77A-A4A3BE151F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D485CEF3-DFCC-42E6-94F2-CD5A5629A5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US14 Sprint 4 " sheetId="24" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>V2</t>
+  </si>
+  <si>
+    <t>claris</t>
   </si>
 </sst>
 </file>
@@ -1176,74 +1179,74 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2157,31 +2160,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6E083A-5555-419D-B1A5-AFD7E800F2F5}">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="67" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="240.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="240.109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="116"/>
+      <c r="C1" s="129"/>
       <c r="D1" s="38"/>
       <c r="E1" s="36"/>
       <c r="F1" s="40"/>
@@ -2192,29 +2195,29 @@
       <c r="K1" s="10"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="117"/>
+      <c r="C2" s="124"/>
       <c r="D2" s="13"/>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="117"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="84"/>
-      <c r="H2" s="117" t="s">
+      <c r="H2" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="107" t="s">
+      <c r="I2" s="124"/>
+      <c r="J2" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="108"/>
+      <c r="K2" s="125"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="22" t="s">
         <v>5</v>
@@ -2244,7 +2247,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="45" t="s">
         <v>10</v>
@@ -2272,7 +2275,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="24" t="s">
         <v>16</v>
@@ -2300,7 +2303,7 @@
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="27" t="s">
         <v>17</v>
@@ -2328,26 +2331,26 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="109"/>
+      <c r="C7" s="126"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="109"/>
+      <c r="F7" s="126"/>
       <c r="G7" s="85"/>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="109"/>
+      <c r="I7" s="126"/>
       <c r="J7"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="58" t="s">
         <v>24</v>
@@ -2373,7 +2376,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="46"/>
       <c r="C9" s="55"/>
@@ -2395,7 +2398,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
@@ -2411,7 +2414,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2427,7 +2430,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="68"/>
       <c r="B12" s="12"/>
       <c r="C12" s="52"/>
@@ -2440,7 +2443,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="69" t="s">
         <v>27</v>
       </c>
@@ -2475,41 +2478,41 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="66" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="118">
+    <row r="14" spans="1:12" s="66" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="107">
         <v>1</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="121" t="s">
+      <c r="C14" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="123" t="s">
+      <c r="D14" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="124"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="127"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="116"/>
       <c r="I14" s="81"/>
       <c r="J14" s="81"/>
       <c r="K14" s="82"/>
     </row>
-    <row r="15" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="122"/>
+    <row r="15" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="107"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="80" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="110" t="s">
+      <c r="F15" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="113" t="s">
+      <c r="G15" s="120" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="75" t="s">
@@ -2521,7 +2524,7 @@
       </c>
       <c r="K15" s="78"/>
     </row>
-    <row r="16" spans="1:12" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="93">
         <v>2</v>
       </c>
@@ -2537,8 +2540,8 @@
       <c r="E16" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="111"/>
-      <c r="G16" s="114"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="100" t="s">
         <v>39</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="77" customFormat="1" ht="291.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" s="77" customFormat="1" ht="291.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="92">
         <v>3</v>
       </c>
@@ -2566,8 +2569,8 @@
       <c r="E17" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="112"/>
-      <c r="G17" s="115"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="102" t="s">
         <v>41</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="98" customFormat="1" ht="302.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" s="98" customFormat="1" ht="302.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="90"/>
       <c r="B18"/>
       <c r="C18" s="73"/>
@@ -2619,28 +2622,28 @@
       <c r="AN18"/>
       <c r="AO18" s="8"/>
     </row>
-    <row r="19" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="117"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="107" t="s">
+      <c r="E19" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="117"/>
+      <c r="F19" s="124"/>
       <c r="G19" s="84"/>
-      <c r="H19" s="117" t="s">
+      <c r="H19" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="117"/>
-      <c r="J19" s="107" t="s">
+      <c r="I19" s="124"/>
+      <c r="J19" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="108"/>
-    </row>
-    <row r="20" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="K19" s="125"/>
+    </row>
+    <row r="20" spans="1:41" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="22" t="s">
         <v>5</v>
@@ -2669,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="45" t="s">
         <v>10</v>
@@ -2696,7 +2699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="24" t="s">
         <v>16</v>
@@ -2723,7 +2726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="27" t="s">
         <v>17</v>
@@ -2750,25 +2753,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="109"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="128" t="s">
+      <c r="E24" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="129"/>
+      <c r="F24" s="128"/>
       <c r="G24" s="85"/>
-      <c r="H24" s="109" t="s">
+      <c r="H24" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="109"/>
+      <c r="I24" s="126"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="58" t="s">
         <v>24</v>
@@ -2791,7 +2794,7 @@
       <c r="J25" s="43"/>
       <c r="K25" s="34"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="46"/>
       <c r="C26" s="55"/>
@@ -2799,7 +2802,9 @@
       <c r="E26" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="59"/>
+      <c r="F26" s="59" t="s">
+        <v>60</v>
+      </c>
       <c r="G26" s="85"/>
       <c r="H26" s="63" t="s">
         <v>14</v>
@@ -2810,7 +2815,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
@@ -2825,7 +2830,7 @@
       <c r="J27" s="21"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -2840,7 +2845,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" s="68"/>
       <c r="B29" s="12"/>
       <c r="C29" s="52"/>
@@ -2853,7 +2858,7 @@
       <c r="J29" s="14"/>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="69" t="s">
         <v>27</v>
       </c>
@@ -2888,41 +2893,41 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="118">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A31" s="107">
         <v>1</v>
       </c>
-      <c r="B31" s="119" t="s">
+      <c r="B31" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="121" t="s">
+      <c r="C31" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="123" t="s">
+      <c r="D31" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="124"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="126"/>
-      <c r="H31" s="127"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="116"/>
       <c r="I31" s="81"/>
       <c r="J31" s="81"/>
       <c r="K31" s="82"/>
     </row>
-    <row r="32" spans="1:41" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="118"/>
-      <c r="B32" s="120"/>
-      <c r="C32" s="122"/>
+    <row r="32" spans="1:41" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="107"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="111"/>
       <c r="D32" s="80" t="s">
         <v>47</v>
       </c>
       <c r="E32" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="110" t="s">
+      <c r="F32" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="113" t="s">
+      <c r="G32" s="120" t="s">
         <v>38</v>
       </c>
       <c r="H32" s="105" t="s">
@@ -2934,7 +2939,7 @@
       </c>
       <c r="K32" s="78"/>
     </row>
-    <row r="33" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="93">
         <v>2</v>
       </c>
@@ -2950,8 +2955,8 @@
       <c r="E33" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="111"/>
-      <c r="G33" s="114"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="121"/>
       <c r="H33" s="100" t="s">
         <v>39</v>
       </c>
@@ -2961,7 +2966,7 @@
       </c>
       <c r="K33" s="80"/>
     </row>
-    <row r="34" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="92">
         <v>3</v>
       </c>
@@ -2977,8 +2982,8 @@
       <c r="E34" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="112"/>
-      <c r="G34" s="115"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="122"/>
       <c r="H34" s="105" t="s">
         <v>41</v>
       </c>
@@ -2990,20 +2995,12 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
@@ -3013,12 +3010,20 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="G32:G34"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15:J17 H15:H18 J32:J34 H32:H34" xr:uid="{654A6606-3A32-42A1-A977-31B0EC5D53E6}">

</xml_diff>